<commit_message>
Updated template definitions to include help field
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="1035A4BBE638" lockStructure="1"/>
+  <workbookProtection workbookPassword="10EB1F471032" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -30442,7 +30442,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="1035A4BBE638"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10EB1F471032"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>

<commit_message>
#1281 Updated schema output to include AdditionalUEIs schemas
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="10EB1F471032" lockStructure="1"/>
+  <workbookProtection workbookPassword="4A32EFBF6414" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -30442,7 +30442,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10EB1F471032"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4A32EFBF6414"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>

<commit_message>
Updated build, fixed parse/render
1. The top-level Makefile now does everything front-to-back.
2. Added `merged_unreachable` as a NT, which was not handled before.

For 1, this now regenerates JSON source documents (program names, ALNs),
which come from the DB. Eventually, we will likely pull from our DB via
API to generate these lists. (Or, something.) For now, we procress data
from Census extracted from their dumps.

For 2, this wasn't handled becuase the sheet I was working with did not
have this field/type. I added it, parsed it, and incorporated it into
the script. (`merged_unreachable` was already in `render.py`, but
`parse` was not handling it correctly. Given that `parse.py` was new,
this makes sense to me.)
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="10EB1F471032" lockStructure="1"/>
+  <workbookProtection workbookPassword="B71253A02AE2" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -30442,7 +30442,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10EB1F471032"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="B71253A02AE2"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>
@@ -39441,17 +39441,14 @@
     <mergeCell ref="G111:H111"/>
     <mergeCell ref="A1615:B1615"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation sqref="A4:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
+  <dataValidations count="3">
+    <dataValidation sqref="A4:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A4), AND(LEN($A4) = 8, LEFT($A4, 2) = "20", ISNUMBER(MID($A4, 3, 2) * 1), MID($A4, 5, 1) = "-", ISNUMBER(RIGHT($A4, 3) * 1)))</formula1>
-    </dataValidation>
-    <dataValidation sqref="G4:G3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must by Y or N" error="Entries must be Y or N in this column" type="list">
-      <formula1>"Y,N"</formula1>
     </dataValidation>
     <dataValidation sqref="G4:G3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Y/N" error="Must be 'Y' or 'N'" type="list">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated workbooks. No other changes.
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="B71253A02AE2" lockStructure="1"/>
+  <workbookProtection workbookPassword="4176FC606BC" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -30442,7 +30442,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="B71253A02AE2"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4176FC606BC"/>
   <mergeCells count="8996">
     <mergeCell ref="A1310:B1310"/>
     <mergeCell ref="G2565:H2565"/>

</xml_diff>

<commit_message>
#1383 Regenerated workbooks to make sure nothing broke
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="AE8701FA081" lockStructure="1"/>
+  <workbookProtection workbookPassword="93E9BE9C69" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15459,7 +15459,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="AE8701FA081"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="93E9BE9C69"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -15500,7 +15500,7 @@
       <c r="A2" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="AE8701FA081"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="93E9BE9C69"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1383 fixed a wrong formula and regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="93E9BE9C69" lockStructure="1"/>
+  <workbookProtection workbookPassword="8537CD27259" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -15459,7 +15459,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="93E9BE9C69"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="8537CD27259"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -15500,7 +15500,7 @@
       <c r="A2" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="93E9BE9C69"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="8537CD27259"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1175 Regenarated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="225538E4C536" lockStructure="1"/>
+  <workbookProtection workbookPassword="27230CEACDB8" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="225538E4C536"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27230CEACDB8"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="225538E4C536"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27230CEACDB8"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1175 Renamed award unique identifier and regenated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="2CE8995BBC9F" lockStructure="1"/>
+  <workbookProtection workbookPassword="A060B68AD44" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2CE8995BBC9F"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A060B68AD44"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2CE8995BBC9F"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A060B68AD44"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1513 Updated left over formulas due to column shift and rebuilt output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="A060B68AD44" lockStructure="1"/>
+  <workbookProtection workbookPassword="10E54F7632EA" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A060B68AD44"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10E54F7632EA"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A060B68AD44"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10E54F7632EA"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1513 Regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="10E54F7632EA" lockStructure="1"/>
+  <workbookProtection workbookPassword="BBF55BBE16F" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10E54F7632EA"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="BBF55BBE16F"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10E54F7632EA"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="BBF55BBE16F"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1435 Regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="A060B68AD44" lockStructure="1"/>
+  <workbookProtection workbookPassword="285717656DC2" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A060B68AD44"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="285717656DC2"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A060B68AD44"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="285717656DC2"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1435 Added missing cluster name
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="28187F2E65D9" lockStructure="1"/>
+  <workbookProtection workbookPassword="40707080B7DF" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="28187F2E65D9"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="40707080B7DF"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="28187F2E65D9"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="40707080B7DF"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
update lots of validation items, consistify property names
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="273276DA3AB" lockStructure="1"/>
+  <workbookProtection workbookPassword="105B8D5798D9" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="273276DA3AB"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="105B8D5798D9"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="273276DA3AB"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="105B8D5798D9"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
catchup broke uniform guidance tests. updating workbooks might fix CI
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="105B8D5798D9" lockStructure="1"/>
+  <workbookProtection workbookPassword="16FFFB1496024" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="105B8D5798D9"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="16FFFB1496024"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="105B8D5798D9"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="16FFFB1496024"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
Secondary auditors workbook (#1331)
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="BBF55BBE16F" lockStructure="1"/>
+  <workbookProtection workbookPassword="16FFFB1496024" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="BBF55BBE16F"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="16FFFB1496024"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="BBF55BBE16F"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="16FFFB1496024"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1431 Regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="BBF55BBE16F" lockStructure="1"/>
+  <workbookProtection workbookPassword="2961FC04FE11" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="BBF55BBE16F"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2961FC04FE11"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="BBF55BBE16F"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2961FC04FE11"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1435 Utilized input parameters and regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="217F5F82C1DC9" lockStructure="1"/>
+  <workbookProtection workbookPassword="21D8EA2D187B" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="217F5F82C1DC9"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="217F5F82C1DC9"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1431 Excluded AWARD-0000 from award reference and regenerated output files + updated branch with latest changes from main
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="8638DD71F58" lockStructure="1"/>
+  <workbookProtection workbookPassword="2450964A7363" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="8638DD71F58"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2450964A7363"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="8638DD71F58"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2450964A7363"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1431 Updated custom error message for compliance requirement types and regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="2450964A7363" lockStructure="1"/>
+  <workbookProtection workbookPassword="169E50341FB7" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2450964A7363"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="169E50341FB7"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="2450964A7363"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="169E50341FB7"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
Jmm/gfac dissemination model (#1598)
* Do dissemination.SecondaryAuditor

* Add audit_info to dissemination

* checkout main schemas
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="169E50341FB7" lockStructure="1"/>
+  <workbookProtection workbookPassword="21D8EA2D187B" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="169E50341FB7"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="169E50341FB7"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
test coversheet using single_cells
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="21D8EA2D187B" lockStructure="1"/>
+  <workbookProtection workbookPassword="23A62C37BDC5" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="23A62C37BDC5"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="23A62C37BDC5"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
Updated passthrough entity column format
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="21D8EA2D187B" lockStructure="1"/>
+  <workbookProtection workbookPassword="5824C986CA3" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="5824C986CA3"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="21D8EA2D187B"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="5824C986CA3"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
add meta-cell type and apply to all workbooks
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-template.xlsx
@@ -2,19 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="23A62C37BDC5" lockStructure="1"/>
+  <workbookProtection workbookPassword="5F129DAAB5F6" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Form" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="UEI" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="UEI" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Form" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="reference_number">'Form'!$A$2:$A$3000</definedName>
     <definedName name="planned_action">'Form'!$B$2:$B$3000</definedName>
     <definedName name="contains_chart_or_table">'Form'!$C$2:$C$3000</definedName>
-    <definedName name="auditee_uei">'UEI'!$A$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -65,15 +64,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
   </cellXfs>
@@ -436,6 +432,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="5F129DAAB5F6"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -31843,7 +31858,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="23A62C37BDC5"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="5F129DAAB5F6"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31854,42 +31869,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="36" customWidth="1" min="1" max="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="48" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Auditee UEI</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="23A62C37BDC5"/>
-  <dataValidations count="1">
-    <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
-      <formula1>12</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>